<commit_message>
Checked design rules. Made gerber and drill
</commit_message>
<xml_diff>
--- a/Piezo BOM.xlsx
+++ b/Piezo BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>Description</t>
   </si>
@@ -102,12 +102,6 @@
     <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/6792039/</t>
   </si>
   <si>
-    <t>http://china.rs-online.com/web/p/pcb-sockets/1216946/</t>
-  </si>
-  <si>
-    <t>5 pin female header</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -136,6 +130,54 @@
   </si>
   <si>
     <t>Should be as close as possible</t>
+  </si>
+  <si>
+    <t>Positions on board</t>
+  </si>
+  <si>
+    <t>DaC, Cref, Ca, Cd, Cc, Cb</t>
+  </si>
+  <si>
+    <t>Rdv1, Rdv2</t>
+  </si>
+  <si>
+    <t>Cf</t>
+  </si>
+  <si>
+    <t>Ra1, Rb1, Rc1, Rd1, Rfa, Rfd, Rfc, Rfb</t>
+  </si>
+  <si>
+    <t>DAC1</t>
+  </si>
+  <si>
+    <t>&lt;Unlabelled&gt;</t>
+  </si>
+  <si>
+    <t>RAGm, RAGp</t>
+  </si>
+  <si>
+    <t>RLAm, RLAp</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>Ra2, Rb2, Rc2, Rd2</t>
+  </si>
+  <si>
+    <t>LmC, LpC, ViC, VoC, OC</t>
+  </si>
+  <si>
+    <t>BmC, BpC</t>
+  </si>
+  <si>
+    <t>Piezos</t>
+  </si>
+  <si>
+    <t>5 pin male header</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/pcb-headers/2518121/?searchTerm=W81105T3825RC&amp;relevancy-data=636F3D3226696E3D4931384E4B6E6F776E41734D504E266C753D7A68266D6D3D6D61746368616C6C7061727469616C26706D3D5E5B5C772D5C2E2F252C5D2B2426706F3D313326736E3D592673743D4B4559574F52445F53494E474C455F414C5048415F4E554D455249432677633D424F5448267573743D57383131303554333832355243267374613D5738313130355433383235524326</t>
   </si>
 </sst>
 </file>
@@ -165,12 +207,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -186,7 +234,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -198,6 +246,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -513,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:D16"/>
+  <dimension ref="A3:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,23 +577,27 @@
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="40.28515625" customWidth="1"/>
     <col min="4" max="4" width="37.5703125" customWidth="1"/>
+    <col min="5" max="5" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -552,10 +608,13 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -566,10 +625,13 @@
         <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -580,10 +642,13 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -594,10 +659,13 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -607,8 +675,11 @@
       <c r="C8" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -618,8 +689,11 @@
       <c r="C9" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -630,10 +704,13 @@
         <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -644,10 +721,13 @@
         <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -658,10 +738,13 @@
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -672,10 +755,13 @@
         <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="E13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -686,10 +772,13 @@
         <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="E14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -700,18 +789,24 @@
         <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="E15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>27</v>
+        <v>52</v>
+      </c>
+      <c r="E16" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -728,9 +823,8 @@
     <hyperlink ref="C14" r:id="rId10"/>
     <hyperlink ref="C15" r:id="rId11"/>
     <hyperlink ref="C13" r:id="rId12"/>
-    <hyperlink ref="C16" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
checked BOM and zipped everything up
</commit_message>
<xml_diff>
--- a/Piezo BOM.xlsx
+++ b/Piezo BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>Description</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>http://china.rs-online.com/web/p/pcb-headers/2518121/?searchTerm=W81105T3825RC&amp;relevancy-data=636F3D3226696E3D4931384E4B6E6F776E41734D504E266C753D7A68266D6D3D6D61746368616C6C7061727469616C26706D3D5E5B5C772D5C2E2F252C5D2B2426706F3D313326736E3D592673743D4B4559574F52445F53494E474C455F414C5048415F4E554D455249432677633D424F5448267573743D57383131303554333832355243267374613D5738313130355433383235524326</t>
+  </si>
+  <si>
+    <t>mounted so that pin 1 is next to the dot</t>
   </si>
 </sst>
 </file>
@@ -568,7 +571,7 @@
   <dimension ref="A3:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,7 +579,7 @@
     <col min="1" max="1" width="32.28515625" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="40.28515625" customWidth="1"/>
-    <col min="4" max="4" width="37.5703125" customWidth="1"/>
+    <col min="4" max="4" width="60.42578125" customWidth="1"/>
     <col min="5" max="5" width="39" customWidth="1"/>
   </cols>
   <sheetData>
@@ -688,6 +691,9 @@
       </c>
       <c r="C9" s="4" t="s">
         <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>53</v>
       </c>
       <c r="E9" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Piezo BOM was missing some parts, wrong parts...
</commit_message>
<xml_diff>
--- a/Piezo BOM.xlsx
+++ b/Piezo BOM.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
   <si>
     <t>Description</t>
   </si>
@@ -69,15 +69,9 @@
     <t>http://china.rs-online.com/web/p/ceramic-multilayer-capacitors/6911161/</t>
   </si>
   <si>
-    <t>http://china.rs-online.com/web/p/ceramic-multilayer-capacitors/7236644/</t>
-  </si>
-  <si>
     <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/6791569/</t>
   </si>
   <si>
-    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/6789667/</t>
-  </si>
-  <si>
     <t>http://china.rs-online.com/web/p/general-purpose-dacs/8065471/</t>
   </si>
   <si>
@@ -87,21 +81,9 @@
     <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/2230691/</t>
   </si>
   <si>
-    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/7169715/</t>
-  </si>
-  <si>
-    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/8145889/</t>
-  </si>
-  <si>
-    <t>http://china.rs-online.com/web/p/ceramic-multilayer-capacitors/8467293/</t>
-  </si>
-  <si>
     <t>http://china.rs-online.com/web/p/ceramic-multilayer-capacitors/2644371/</t>
   </si>
   <si>
-    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/6792039/</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -181,6 +163,30 @@
   </si>
   <si>
     <t>mounted so that pin 1 is next to the dot</t>
+  </si>
+  <si>
+    <t>LM324AD</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/operational-amplifiers/5171876/</t>
+  </si>
+  <si>
+    <t>LM324</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/2230562/</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/ceramic-multilayer-capacitors/7236098/</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/7087004/</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/2230427/</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/6791263/</t>
   </si>
 </sst>
 </file>
@@ -568,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E16"/>
+  <dimension ref="A3:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,10 +600,10 @@
         <v>14</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -611,10 +617,10 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -625,13 +631,13 @@
         <v>2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -642,13 +648,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -659,13 +665,13 @@
         <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -676,10 +682,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -690,13 +696,13 @@
         <v>1</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -707,13 +713,13 @@
         <v>2</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -724,13 +730,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -741,13 +747,13 @@
         <v>1</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -758,13 +764,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -775,13 +781,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -792,45 +798,53 @@
         <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E15" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1"/>
-    <hyperlink ref="C6" r:id="rId2"/>
-    <hyperlink ref="C7" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C8" r:id="rId5"/>
-    <hyperlink ref="C9" r:id="rId6"/>
-    <hyperlink ref="C10" r:id="rId7"/>
-    <hyperlink ref="C11" r:id="rId8"/>
-    <hyperlink ref="C12" r:id="rId9"/>
-    <hyperlink ref="C14" r:id="rId10"/>
-    <hyperlink ref="C15" r:id="rId11"/>
-    <hyperlink ref="C13" r:id="rId12"/>
+    <hyperlink ref="C7" r:id="rId2"/>
+    <hyperlink ref="C8" r:id="rId3"/>
+    <hyperlink ref="C9" r:id="rId4"/>
+    <hyperlink ref="C10" r:id="rId5"/>
+    <hyperlink ref="C15" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added jumper and resistor between VRef and +5V Altered BOM parts so that Cf and R14 (for LTC3260) match datasheet Remade Gerber bits Sent to Donny
</commit_message>
<xml_diff>
--- a/Piezo BOM.xlsx
+++ b/Piezo BOM.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,9 +30,6 @@
     <t>10k surface mount resistors 0805</t>
   </si>
   <si>
-    <t>1.5uF surface mount capacitors 0805</t>
-  </si>
-  <si>
     <t>5k surface mount resistors 0805</t>
   </si>
   <si>
@@ -48,9 +45,6 @@
     <t>800k surface mount resistors 0805</t>
   </si>
   <si>
-    <t>1k surface mount resistors 0805</t>
-  </si>
-  <si>
     <t>30k surface mount resistors 0805</t>
   </si>
   <si>
@@ -93,9 +87,6 @@
     <t>Can vary from 10 to 50kOhm</t>
   </si>
   <si>
-    <t>Can be anything from 1.5uF to 5uF</t>
-  </si>
-  <si>
     <t>Can vary from 4.8k to 5.2k</t>
   </si>
   <si>
@@ -105,9 +96,6 @@
     <t>can vary from 780k to 820k</t>
   </si>
   <si>
-    <t>can vary from 900 to 1.2k</t>
-  </si>
-  <si>
     <t>can vary from 28k to 32k</t>
   </si>
   <si>
@@ -120,9 +108,6 @@
     <t>DaC, Cref, Ca, Cd, Cc, Cb</t>
   </si>
   <si>
-    <t>Rdv1, Rdv2</t>
-  </si>
-  <si>
     <t>Cf</t>
   </si>
   <si>
@@ -177,16 +162,31 @@
     <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/2230562/</t>
   </si>
   <si>
-    <t>http://china.rs-online.com/web/p/ceramic-multilayer-capacitors/7236098/</t>
-  </si>
-  <si>
     <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/7087004/</t>
   </si>
   <si>
-    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/2230427/</t>
-  </si>
-  <si>
     <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/6791263/</t>
+  </si>
+  <si>
+    <t>Rdv1, Rdv2,Rdr</t>
+  </si>
+  <si>
+    <t>200k surface mount resistor 0805</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/surface-mount-fixed-resistors/6791064/</t>
+  </si>
+  <si>
+    <t>has to be 200k</t>
+  </si>
+  <si>
+    <t>http://china.rs-online.com/web/p/ceramic-multilayer-capacitors/4515770/</t>
+  </si>
+  <si>
+    <t>Must be 1uF</t>
+  </si>
+  <si>
+    <t>1uF surface mount capacitors 0805</t>
   </si>
 </sst>
 </file>
@@ -577,7 +577,7 @@
   <dimension ref="A3:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,16 +594,16 @@
         <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -614,13 +614,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -628,211 +628,211 @@
         <v>2</v>
       </c>
       <c r="B5" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="2">
         <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="2">
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2">
         <v>2</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="2">
         <v>2</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="B12" s="2">
         <v>1</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>54</v>
+      <c r="C12" t="s">
+        <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2">
         <v>4</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B14" s="2">
         <v>5</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" s="2">
         <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B16" s="2">
         <v>1</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B17" s="2">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>